<commit_message>
add district level, service layer
</commit_message>
<xml_diff>
--- a/Indonesia/input.xlsx
+++ b/Indonesia/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crops\crawler\Indonesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D0F2E5-40A6-489A-BE10-E9BFFCA59D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67780656-717F-43A2-A30A-D4B585487147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2178" yWindow="3013" windowWidth="17425" windowHeight="9039" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11810" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Subsection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Crop</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +52,26 @@
   </si>
   <si>
     <t>PRODUKSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subsection(agriculture product)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>State</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kabupaten</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aceh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -63,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +93,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFE3E3E3"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,57 +404,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>2016</v>
-      </c>
-      <c r="E2">
-        <v>2022</v>
+      <c r="F2">
+        <v>1970</v>
+      </c>
+      <c r="G2">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add merge and rearrange
</commit_message>
<xml_diff>
--- a/Indonesia/input.xlsx
+++ b/Indonesia/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22410" windowHeight="9958"/>
+    <workbookView windowWidth="12488" windowHeight="9245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Level</t>
   </si>
@@ -53,16 +53,34 @@
     <t>Kabupaten</t>
   </si>
   <si>
-    <t>Jawa Tengah</t>
-  </si>
-  <si>
-    <t>KACANG HIJAU</t>
-  </si>
-  <si>
-    <t>Tanaman Pangan</t>
+    <t>Sulawesi Barat</t>
+  </si>
+  <si>
+    <t>KELAPA</t>
+  </si>
+  <si>
+    <t>Perkebunan</t>
+  </si>
+  <si>
+    <t>PRODUKSI</t>
+  </si>
+  <si>
+    <t>Kalimantan Barat</t>
+  </si>
+  <si>
+    <t>TOMAT</t>
+  </si>
+  <si>
+    <t>Hortikultura</t>
   </si>
   <si>
     <t>LUAS PANEN</t>
+  </si>
+  <si>
+    <t>Kepulauan Riau</t>
+  </si>
+  <si>
+    <t>LUAS AREAL</t>
   </si>
 </sst>
 </file>
@@ -705,8 +723,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1057,34 +1077,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="10.5504587155963" customWidth="1"/>
+    <col min="2" max="2" width="32.9908256880734" customWidth="1"/>
+    <col min="3" max="3" width="16.1100917431193" customWidth="1"/>
+    <col min="4" max="4" width="13.0917431192661" customWidth="1"/>
+    <col min="5" max="5" width="11.8715596330275" customWidth="1"/>
+    <col min="6" max="6" width="13.0917431192661" customWidth="1"/>
+    <col min="7" max="7" width="10.651376146789" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1108,6 +1137,98 @@
         <v>1970</v>
       </c>
       <c r="G2" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1970</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="1" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1970</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1970</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1970</v>
+      </c>
+      <c r="G6" s="3">
         <v>2024</v>
       </c>
     </row>

</xml_diff>